<commit_message>
login page added. confirmation page restyled.
</commit_message>
<xml_diff>
--- a/2020-05.xlsx
+++ b/2020-05.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="12" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="16" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="2020-05-10" sheetId="1" r:id="rId4"/>
@@ -20,6 +20,10 @@
     <sheet name="2020-05-20 3" sheetId="11" r:id="rId14"/>
     <sheet name="2020-05-2020-05-11" sheetId="12" r:id="rId15"/>
     <sheet name="2020-05-20 4" sheetId="13" r:id="rId16"/>
+    <sheet name="2020-05-20 5" sheetId="14" r:id="rId17"/>
+    <sheet name="2020-05-2020-05-26" sheetId="15" r:id="rId18"/>
+    <sheet name="2020-05-28" sheetId="16" r:id="rId19"/>
+    <sheet name="2020-05-2020-05-29" sheetId="17" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>記入者</t>
   </si>
@@ -348,6 +352,24 @@
   </si>
   <si>
     <t>11円</t>
+  </si>
+  <si>
+    <t>2020-05-2020-05-26</t>
+  </si>
+  <si>
+    <t>4円</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>2020-05-28</t>
+  </si>
+  <si>
+    <t>様</t>
+  </si>
+  <si>
+    <t>2020-05-2020-05-29</t>
   </si>
 </sst>
 </file>
@@ -3256,6 +3278,2458 @@
   </sheetPr>
   <dimension ref="A1:M39"/>
   <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A35" sqref="A35:L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="J9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="J12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="2"/>
+      <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="2">
+        <v>500</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="2">
+        <v>200</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32"/>
+      <c r="K32"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="C2:C2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="A6:A6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:L39"/>
+  </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:M39"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A35" sqref="A35:L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="J9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="J12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="2"/>
+      <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="2">
+        <v>500</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="2">
+        <v>200</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32"/>
+      <c r="K32"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="C2:C2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="A6:A6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:L39"/>
+  </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:M39"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A35" sqref="A35:L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="J9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="J12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="2"/>
+      <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="2">
+        <v>500</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="2">
+        <v>200</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32"/>
+      <c r="K32"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="C2:C2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="A6:A6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:L39"/>
+  </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:M39"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A35" sqref="A35:L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>300</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>300</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="J9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="J12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="2"/>
+      <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="2">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="2">
+        <v>3</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="2">
+        <v>3</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="2">
+        <v>3</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="2">
+        <v>3</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="2">
+        <v>3</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="2">
+        <v>3</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" t="s">
+        <v>56</v>
+      </c>
+      <c r="K31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32"/>
+      <c r="K32"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="C2:C2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="A6:A6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:L39"/>
+  </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:M39"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A35" sqref="A35:L39"/>
     </sheetView>
@@ -3267,7 +5741,7 @@
         <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -3275,7 +5749,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -3343,13 +5817,13 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>99</v>
+      <c r="H6" s="2">
+        <v>1</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
-        <v>99</v>
+      <c r="K6" s="2">
+        <v>1</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -3366,13 +5840,13 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>100</v>
+      <c r="H7" s="2">
+        <v>1</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>100</v>
+      <c r="K7" s="2">
+        <v>1</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -3613,10 +6087,10 @@
         <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E22" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:13">

</xml_diff>